<commit_message>
Sprint 3 Review and burnup, + final documentation
</commit_message>
<xml_diff>
--- a/Sprint 3 Burnup Chart.xlsx
+++ b/Sprint 3 Burnup Chart.xlsx
@@ -171,11 +171,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1144563568"/>
-        <c:axId val="1536864106"/>
+        <c:axId val="435221719"/>
+        <c:axId val="613256973"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1144563568"/>
+        <c:axId val="435221719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -195,10 +195,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1536864106"/>
+        <c:crossAx val="613256973"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1536864106"/>
+        <c:axId val="613256973"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -234,7 +234,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1144563568"/>
+        <c:crossAx val="435221719"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -306,6 +306,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -339,8 +342,8 @@
       <c r="B2" s="2">
         <v>35.0</v>
       </c>
-      <c r="C2">
-        <v>0.0</v>
+      <c r="C2" s="2">
+        <v>1.0</v>
       </c>
       <c r="D2" s="2">
         <v>0.0</v>
@@ -353,8 +356,8 @@
       <c r="B3" s="2">
         <v>35.0</v>
       </c>
-      <c r="C3">
-        <v>0.0</v>
+      <c r="C3" s="2">
+        <v>3.0</v>
       </c>
       <c r="D3" s="2">
         <v>3.0</v>
@@ -367,8 +370,8 @@
       <c r="B4" s="2">
         <v>35.0</v>
       </c>
-      <c r="C4">
-        <v>0.0</v>
+      <c r="C4" s="2">
+        <v>5.0</v>
       </c>
       <c r="D4" s="2">
         <v>6.0</v>
@@ -381,8 +384,8 @@
       <c r="B5" s="2">
         <v>35.0</v>
       </c>
-      <c r="C5">
-        <v>0.0</v>
+      <c r="C5" s="2">
+        <v>8.0</v>
       </c>
       <c r="D5" s="2">
         <v>9.0</v>
@@ -395,8 +398,8 @@
       <c r="B6" s="2">
         <v>35.0</v>
       </c>
-      <c r="C6">
-        <v>0.0</v>
+      <c r="C6" s="2">
+        <v>12.0</v>
       </c>
       <c r="D6" s="2">
         <v>11.0</v>
@@ -409,8 +412,8 @@
       <c r="B7" s="2">
         <v>35.0</v>
       </c>
-      <c r="C7">
-        <v>0.0</v>
+      <c r="C7" s="2">
+        <v>15.0</v>
       </c>
       <c r="D7" s="2">
         <v>14.0</v>
@@ -423,8 +426,8 @@
       <c r="B8" s="2">
         <v>35.0</v>
       </c>
-      <c r="C8">
-        <v>0.0</v>
+      <c r="C8" s="2">
+        <v>18.0</v>
       </c>
       <c r="D8" s="2">
         <v>16.0</v>
@@ -437,8 +440,8 @@
       <c r="B9" s="2">
         <v>35.0</v>
       </c>
-      <c r="C9">
-        <v>0.0</v>
+      <c r="C9" s="2">
+        <v>21.0</v>
       </c>
       <c r="D9" s="2">
         <v>18.0</v>
@@ -451,8 +454,8 @@
       <c r="B10" s="2">
         <v>35.0</v>
       </c>
-      <c r="C10">
-        <v>0.0</v>
+      <c r="C10" s="2">
+        <v>24.0</v>
       </c>
       <c r="D10" s="2">
         <v>20.0</v>
@@ -465,8 +468,8 @@
       <c r="B11" s="2">
         <v>35.0</v>
       </c>
-      <c r="C11">
-        <v>0.0</v>
+      <c r="C11" s="2">
+        <v>27.0</v>
       </c>
       <c r="D11" s="2">
         <v>24.0</v>
@@ -479,8 +482,8 @@
       <c r="B12" s="2">
         <v>35.0</v>
       </c>
-      <c r="C12">
-        <v>0.0</v>
+      <c r="C12" s="2">
+        <v>29.0</v>
       </c>
       <c r="D12" s="2">
         <v>28.0</v>
@@ -493,8 +496,8 @@
       <c r="B13" s="2">
         <v>35.0</v>
       </c>
-      <c r="C13">
-        <v>0.0</v>
+      <c r="C13" s="2">
+        <v>30.0</v>
       </c>
       <c r="D13" s="2">
         <v>30.0</v>
@@ -508,7 +511,7 @@
         <v>35.0</v>
       </c>
       <c r="C14" s="2">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="D14" s="2">
         <v>32.0</v>
@@ -522,7 +525,7 @@
         <v>35.0</v>
       </c>
       <c r="C15" s="2">
-        <v>0.0</v>
+        <v>38.0</v>
       </c>
       <c r="D15" s="2">
         <v>35.0</v>
@@ -1514,6 +1517,9 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>